<commit_message>
ema trader 3 - dev
</commit_message>
<xml_diff>
--- a/ema_len calc.xlsx
+++ b/ema_len calc.xlsx
@@ -28,13 +28,13 @@
     <t xml:space="preserve">candle_size</t>
   </si>
   <si>
-    <t xml:space="preserve">short</t>
-  </si>
-  <si>
-    <t xml:space="preserve">long</t>
-  </si>
-  <si>
-    <t xml:space="preserve">additional_ema_len</t>
+    <t xml:space="preserve">sema</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lema</t>
+  </si>
+  <si>
+    <t xml:space="preserve">slema</t>
   </si>
 </sst>
 </file>
@@ -49,6 +49,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -133,14 +134,14 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.99"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="16.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="16.59"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="5" style="0" width="11.52"/>
   </cols>
   <sheetData>
@@ -171,11 +172,11 @@
         <v>2</v>
       </c>
       <c r="B4" s="0" t="n">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="C4" s="0" t="n">
         <f aca="false">B4*$C$3</f>
-        <v>15000</v>
+        <v>3000</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -183,11 +184,11 @@
         <v>3</v>
       </c>
       <c r="B5" s="0" t="n">
-        <v>200</v>
+        <v>100</v>
       </c>
       <c r="C5" s="0" t="n">
         <f aca="false">B5*$C$3</f>
-        <v>60000</v>
+        <v>30000</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -195,11 +196,11 @@
         <v>4</v>
       </c>
       <c r="B6" s="0" t="n">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="C6" s="0" t="n">
         <f aca="false">B6*$C$3</f>
-        <v>6000</v>
+        <v>7500</v>
       </c>
     </row>
   </sheetData>

</xml_diff>